<commit_message>
changes from ban keat in wheel force
</commit_message>
<xml_diff>
--- a/Excel excel excel bestnye.xlsx
+++ b/Excel excel excel bestnye.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MEC 3416\ST-23\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SCHOOLING IS FUN\Year 2 sem 2\MEC3416\ST-23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B188BEA-F938-4D2A-89DE-82315623ED2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F108E4A3-2925-4669-AE5A-4A7A9A841914}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{54E2048A-4415-4651-99B5-0EF0CC87E6DB}"/>
+    <workbookView xWindow="2472" yWindow="2472" windowWidth="17280" windowHeight="8964" xr2:uid="{54E2048A-4415-4651-99B5-0EF0CC87E6DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -105,12 +105,6 @@
     <t xml:space="preserve">Friction force </t>
   </si>
   <si>
-    <t>Load for left wheels (only concrete block) (N)</t>
-  </si>
-  <si>
-    <t>Load for right wheels (only concrete block) (N)</t>
-  </si>
-  <si>
     <t>Friction coefficent (static friction only)
 Material: Mild steel</t>
   </si>
@@ -243,6 +237,12 @@
   </si>
   <si>
     <t>(depends on direction of torque)</t>
+  </si>
+  <si>
+    <t>Load for each left wheel (only concrete block) (N)</t>
+  </si>
+  <si>
+    <t>Load for each right wheel (only concrete block) (N)</t>
   </si>
 </sst>
 </file>
@@ -365,9 +365,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -379,6 +376,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -696,14 +696,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5373BFE-1F71-450B-A293-F590D0A3A936}">
   <dimension ref="A1:G197"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.21875" customWidth="1"/>
     <col min="5" max="5" width="38.109375" customWidth="1"/>
@@ -718,7 +718,7 @@
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -812,7 +812,7 @@
     <row r="10" spans="1:7" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1">
         <v>0.19</v>
@@ -821,41 +821,41 @@
     <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="C11" s="1">
-        <v>7627.3349630000002</v>
+        <v>6777.818182</v>
       </c>
       <c r="D11" s="1">
         <f>C11*$C$10</f>
-        <v>1449.1936429700002</v>
+        <v>1287.7854545800001</v>
       </c>
       <c r="E11" s="1">
         <f>D11*$C$13</f>
-        <v>507.2177750395</v>
+        <v>450.72490910300002</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>67</v>
       </c>
       <c r="C12" s="1">
-        <v>4144.6650369999998</v>
+        <v>4994.181818</v>
       </c>
       <c r="D12" s="1">
         <f>C12*$C$10</f>
-        <v>787.48635702999991</v>
+        <v>948.89454541999999</v>
       </c>
       <c r="E12" s="1">
         <f>D12*$C$13</f>
-        <v>275.62022496049997</v>
+        <v>332.11309089699995</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C13" s="1">
         <v>0.35</v>
@@ -864,7 +864,7 @@
     <row r="14" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" s="10">
         <v>0.25</v>
@@ -887,7 +887,7 @@
         <v>18</v>
       </c>
       <c r="C17" s="1">
-        <v>7627.3349630000002</v>
+        <v>6777.818182</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -896,7 +896,7 @@
         <v>19</v>
       </c>
       <c r="C18" s="1">
-        <v>4144.6650369999998</v>
+        <v>4994.181818</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -930,49 +930,49 @@
     </row>
     <row r="26" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="14" t="s">
-        <v>29</v>
+      <c r="A27" s="18" t="s">
+        <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C27" s="1">
         <v>0.35</v>
       </c>
       <c r="E27" s="1">
         <f>C28*C27</f>
-        <v>1014.435550079</v>
+        <v>901.44981820600003</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="14"/>
+      <c r="A28" s="18"/>
       <c r="B28" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C28" s="1">
         <f>D11*2</f>
-        <v>2898.3872859400003</v>
+        <v>2575.5709091600002</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="14" t="s">
-        <v>30</v>
+      <c r="A29" s="18" t="s">
+        <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C29" s="1">
         <f>C27</f>
@@ -980,23 +980,23 @@
       </c>
       <c r="E29" s="1">
         <f>C29*C30</f>
-        <v>551.24044992099994</v>
+        <v>664.2261817939999</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="14"/>
+      <c r="A30" s="18"/>
       <c r="B30" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C30" s="1">
         <f>D12*2</f>
-        <v>1574.9727140599998</v>
+        <v>1897.78909084</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="D31" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E31" s="1">
         <f>E27+E29</f>
@@ -1008,19 +1008,19 @@
     </row>
     <row r="33" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C33" s="11">
         <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="18"/>
+      <c r="A34" s="17"/>
       <c r="B34" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C34" s="11">
         <v>4000</v>
@@ -1029,7 +1029,7 @@
     <row r="35" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="13"/>
       <c r="B35" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C35" s="1">
         <v>0.17499999999999999</v>
@@ -1037,12 +1037,12 @@
     </row>
     <row r="36" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B36" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C36" s="17">
+        <v>56</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" s="16">
         <f>C33</f>
         <v>100</v>
       </c>
@@ -1050,7 +1050,7 @@
     <row r="37" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
       <c r="B37" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C37" s="1">
         <f>C34/C35</f>
@@ -1060,7 +1060,7 @@
     <row r="38" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="B38" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C38" s="1">
         <f>C37</f>
@@ -1071,51 +1071,51 @@
       <c r="A39" s="8"/>
     </row>
     <row r="40" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="16" t="s">
-        <v>34</v>
+      <c r="A40" s="15" t="s">
+        <v>32</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C40" s="1">
         <v>4000</v>
       </c>
-      <c r="E40" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="F40" s="15">
+      <c r="E40" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F40" s="14">
         <v>0.01</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5"/>
       <c r="B41" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C41" s="1">
         <v>0.2</v>
       </c>
-      <c r="E41" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="F41" s="15">
+      <c r="E41" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F41" s="14">
         <v>0.06</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C42" s="1">
         <v>10000</v>
       </c>
-      <c r="E42" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="F42" s="15">
+      <c r="E42" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F42" s="14">
         <f>(E31/C29)/(2*4)</f>
         <v>559.16999999999996</v>
       </c>
@@ -1123,72 +1123,72 @@
     <row r="43" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5"/>
       <c r="B43" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E43" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F43" s="15">
+        <v>65</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F43" s="14">
         <f>PI()*F40^2</f>
         <v>3.1415926535897931E-4</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5"/>
-      <c r="E44" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="F44" s="15">
+      <c r="E44" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F44" s="14">
         <f>PI()*(F40^4)/4</f>
         <v>7.8539816339744827E-9</v>
       </c>
     </row>
     <row r="45" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5"/>
-      <c r="E45" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="F45" s="15">
+      <c r="E45" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F45" s="14">
         <f>(4*F40)/(3*PI())</f>
         <v>4.2441318157838762E-3</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5"/>
-      <c r="E46" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F46" s="15">
+      <c r="E46" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F46" s="14">
         <f>(F43/2)*F45</f>
         <v>6.6666666666666671E-7</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5"/>
-      <c r="E47" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F47" s="15">
+      <c r="E47" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F47" s="14">
         <f xml:space="preserve"> F40</f>
         <v>0.01</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5"/>
-      <c r="E48" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="F48" s="15">
+      <c r="E48" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F48" s="14">
         <f>E31</f>
         <v>1565.6759999999999</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5"/>
-      <c r="E49" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="F49" s="15">
+      <c r="E49" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F49" s="14">
         <f>(F42*F46)/(F44*F47)</f>
         <v>4746382.3748637391</v>
       </c>
@@ -1197,16 +1197,16 @@
       <c r="A50" s="8"/>
     </row>
     <row r="51" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="16" t="s">
-        <v>51</v>
+      <c r="A51" s="15" t="s">
+        <v>49</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E51" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="F51" s="15">
+      <c r="E51" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F51" s="14">
         <v>0.05</v>
       </c>
     </row>
@@ -1215,48 +1215,48 @@
       <c r="B52" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E52" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="F52" s="15"/>
+      <c r="E52" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F52" s="14"/>
     </row>
     <row r="53" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E53" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="F53" s="15"/>
+        <v>57</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F53" s="14"/>
     </row>
     <row r="54" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E54" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="F54" s="15">
+        <v>58</v>
+      </c>
+      <c r="E54" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F54" s="14">
         <f>C17</f>
-        <v>7627.3349630000002</v>
+        <v>6777.818182</v>
       </c>
     </row>
     <row r="55" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5"/>
-      <c r="E55" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F55" s="15">
+      <c r="E55" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F55" s="14">
         <f>E11/F51</f>
-        <v>10144.355500789999</v>
+        <v>9014.4981820600005</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="5"/>
-      <c r="E56" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="F56" s="15">
+      <c r="E56" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F56" s="14">
         <v>0</v>
       </c>
     </row>

</xml_diff>